<commit_message>
Fixing extent null pointer issue
</commit_message>
<xml_diff>
--- a/src/test/resources/com/happiestmind/data/RegressionTests.xlsx
+++ b/src/test/resources/com/happiestmind/data/RegressionTests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>RegressionSearchTest</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>

</xml_diff>